<commit_message>
total per tipe pekerjaan menu kelola penugasan done
</commit_message>
<xml_diff>
--- a/download_contoh_excel/contoh_import_excel.xlsx
+++ b/download_contoh_excel/contoh_import_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\git\auto2000\download_contoh_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF17B759-0537-4F71-B424-088DDA5CDD59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA0C2EC-7D81-42AD-985B-B4F24033B955}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CCCDBD7D-D0D6-4BEE-9085-7683A1027730}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>No. Rangka</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Hendri Susilo</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,8 +158,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,26 +185,18 @@
         <bgColor theme="9" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -222,47 +224,194 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </left>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -273,6 +422,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{12BEA94F-AD1E-4855-A91B-3E4B65546A9C}" name="Table1" displayName="Table1" ref="A1:G6" totalsRowShown="0" tableBorderDxfId="6">
+  <autoFilter ref="A1:G6" xr:uid="{B57B1A2D-44C3-4D06-B3CF-72E3F010FEDC}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{217BF889-24A8-427D-8047-3CFA8DF293D3}" name="No. Rangka" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{C14E87F7-CEDF-4D24-8AE6-6A49FE6E268A}" name="No. Polisi" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DBA7CAC9-F940-4C09-8037-D72D0B60270C}" name="Jenis Kendaraan" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FB417C80-5CB3-42A7-936F-6F9E59B7B45B}" name="Type Pekerjaan" dataDxfId="2" dataCellStyle="Comma [0]"/>
+    <tableColumn id="5" xr3:uid="{16E1A6ED-2338-4AE0-82CF-A00D7F2E99A6}" name="Tanggal Service" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{6C04C95B-8DC3-4317-96A9-C9BD02F1A7D1}" name="Service Advisor" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{22BE4A6E-6838-4287-89A6-1912501CDC47}" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -572,143 +737,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6D666E-7B71-4106-9A2D-6B96F774CD77}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="7">
         <v>43374</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="11">
         <v>43374</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>43374</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="11">
         <v>43374</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>43374</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
if else kelola penugasan
</commit_message>
<xml_diff>
--- a/download_contoh_excel/contoh_import_excel.xlsx
+++ b/download_contoh_excel/contoh_import_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\git\auto2000\download_contoh_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA0C2EC-7D81-42AD-985B-B4F24033B955}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A75C51C-503E-4A0E-8643-19143C9B43B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CCCDBD7D-D0D6-4BEE-9085-7683A1027730}"/>
   </bookViews>
@@ -740,7 +740,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>